<commit_message>
Changed event type on gamedays to "Game".
Have not edited start/end time for gamedays.
</commit_message>
<xml_diff>
--- a/event.xlsx
+++ b/event.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csyers\Documents\Fall 2016\Database Concepts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\ND '16-'17\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5745"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="6">
   <si>
     <t>Event ID</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Practice</t>
+  </si>
+  <si>
+    <t>Game</t>
   </si>
 </sst>
 </file>
@@ -393,13 +396,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -611,9 +614,8 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B15" t="s">
+        <v>5</v>
       </c>
       <c r="C15" s="1">
         <v>42617.770833333336</v>
@@ -626,9 +628,8 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B16" t="s">
+        <v>4</v>
       </c>
       <c r="C16" s="1">
         <v>42618.770833333336</v>
@@ -701,9 +702,8 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B21" t="s">
+        <v>5</v>
       </c>
       <c r="C21" s="1">
         <v>42623.770833333336</v>
@@ -716,9 +716,8 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B22" t="s">
+        <v>4</v>
       </c>
       <c r="C22" s="1">
         <v>42624.770833333336</v>
@@ -806,9 +805,8 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B28" t="s">
+        <v>5</v>
       </c>
       <c r="C28" s="1">
         <v>42630.770833333336</v>
@@ -821,9 +819,8 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B29" t="s">
+        <v>4</v>
       </c>
       <c r="C29" s="1">
         <v>42631.770833333336</v>
@@ -911,9 +908,8 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B35" t="s">
+        <v>5</v>
       </c>
       <c r="C35" s="1">
         <v>42637.770833333336</v>
@@ -926,9 +922,8 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B36" t="s">
+        <v>4</v>
       </c>
       <c r="C36" s="1">
         <v>42638.770833333336</v>
@@ -1016,9 +1011,8 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B42" t="s">
+        <v>5</v>
       </c>
       <c r="C42" s="1">
         <v>42644.770833333336</v>
@@ -1031,9 +1025,8 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B43" t="s">
+        <v>4</v>
       </c>
       <c r="C43" s="1">
         <v>42645.770833333336</v>
@@ -1121,9 +1114,8 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B49" t="s">
+        <v>5</v>
       </c>
       <c r="C49" s="1">
         <v>42651.770833333336</v>
@@ -1136,9 +1128,8 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B50" t="s">
+        <v>4</v>
       </c>
       <c r="C50" s="1">
         <v>42652.770833333336</v>
@@ -1181,9 +1172,8 @@
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B53" t="s">
+        <v>5</v>
       </c>
       <c r="C53" s="1">
         <v>42655.770833333336</v>
@@ -1196,9 +1186,8 @@
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B54" t="s">
+        <v>4</v>
       </c>
       <c r="C54" s="1">
         <v>42656.770833333336</v>
@@ -1226,9 +1215,8 @@
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B56" t="s">
+        <v>5</v>
       </c>
       <c r="C56" s="1">
         <v>42658.770833333336</v>
@@ -1241,9 +1229,8 @@
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B57" t="s">
+        <v>4</v>
       </c>
       <c r="C57" s="1">
         <v>42659.770833333336</v>
@@ -1436,9 +1423,8 @@
       <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70" t="str">
-        <f t="shared" si="0"/>
-        <v>Practice</v>
+      <c r="B70" t="s">
+        <v>5</v>
       </c>
       <c r="C70" s="1">
         <v>42672.770833333336</v>
@@ -1451,9 +1437,8 @@
       <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71" t="str">
-        <f t="shared" ref="B71:B115" si="1">B70</f>
-        <v>Practice</v>
+      <c r="B71" t="s">
+        <v>4</v>
       </c>
       <c r="C71" s="1">
         <v>42673.770833333336</v>
@@ -1467,7 +1452,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B71:B115" si="1">B71</f>
         <v>Practice</v>
       </c>
       <c r="C72" s="1">
@@ -1546,9 +1531,8 @@
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="B77" t="str">
-        <f t="shared" si="1"/>
-        <v>Practice</v>
+      <c r="B77" t="s">
+        <v>5</v>
       </c>
       <c r="C77" s="1">
         <v>42679.770833333336</v>
@@ -1562,9 +1546,8 @@
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
-      <c r="B78" t="str">
-        <f t="shared" si="1"/>
-        <v>Practice</v>
+      <c r="B78" t="s">
+        <v>4</v>
       </c>
       <c r="C78" s="1">
         <v>42680.770833333336</v>
@@ -1658,9 +1641,8 @@
         <f t="shared" si="2"/>
         <v>83</v>
       </c>
-      <c r="B84" t="str">
-        <f t="shared" si="1"/>
-        <v>Practice</v>
+      <c r="B84" t="s">
+        <v>5</v>
       </c>
       <c r="C84" s="1">
         <v>42686.770833333336</v>
@@ -1674,9 +1656,8 @@
         <f t="shared" si="2"/>
         <v>84</v>
       </c>
-      <c r="B85" t="str">
-        <f t="shared" si="1"/>
-        <v>Practice</v>
+      <c r="B85" t="s">
+        <v>4</v>
       </c>
       <c r="C85" s="1">
         <v>42687.770833333336</v>
@@ -1770,9 +1751,8 @@
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="B91" t="str">
-        <f t="shared" si="1"/>
-        <v>Practice</v>
+      <c r="B91" t="s">
+        <v>5</v>
       </c>
       <c r="C91" s="1">
         <v>42693.770833333336</v>
@@ -1786,9 +1766,8 @@
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
-      <c r="B92" t="str">
-        <f t="shared" si="1"/>
-        <v>Practice</v>
+      <c r="B92" t="s">
+        <v>4</v>
       </c>
       <c r="C92" s="1">
         <v>42694.770833333336</v>
@@ -1882,9 +1861,8 @@
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
-      <c r="B98" t="str">
-        <f t="shared" si="1"/>
-        <v>Practice</v>
+      <c r="B98" t="s">
+        <v>5</v>
       </c>
       <c r="C98" s="1">
         <v>42700.770833333336</v>
@@ -1898,9 +1876,8 @@
         <f t="shared" si="2"/>
         <v>98</v>
       </c>
-      <c r="B99" t="str">
-        <f t="shared" si="1"/>
-        <v>Practice</v>
+      <c r="B99" t="s">
+        <v>4</v>
       </c>
       <c r="C99" s="1">
         <v>42701.770833333336</v>

</xml_diff>